<commit_message>
implemented add owners functionality
</commit_message>
<xml_diff>
--- a/resources/cars.xlsx
+++ b/resources/cars.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/378633b9415d47a5/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Techidol solutions\CRM\crm_dashboard\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_F25DC773A252ABDACC1048D8619F5E285BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2525C57-600C-4F2C-A13C-9DCA0967A402}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35E0617-3B1C-4187-9B85-7A6A02A7C82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Brand</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Vehicle Number</t>
-  </si>
-  <si>
     <t>FRV code</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Seater</t>
   </si>
   <si>
-    <t>Rohan</t>
-  </si>
-  <si>
     <t>Land Rover</t>
   </si>
   <si>
@@ -60,53 +54,95 @@
     <t>MP04CT1234</t>
   </si>
   <si>
-    <t>DXLY4260</t>
-  </si>
-  <si>
     <t>MP04CT1235</t>
   </si>
   <si>
-    <t>DXLY4261</t>
-  </si>
-  <si>
     <t>MP04CT1236</t>
   </si>
   <si>
-    <t>DXLY4262</t>
-  </si>
-  <si>
     <t>MP04CT1237</t>
   </si>
   <si>
-    <t>DXLY4263</t>
-  </si>
-  <si>
     <t>MP04CT1238</t>
   </si>
   <si>
-    <t>DXLY4264</t>
-  </si>
-  <si>
     <t>MP04CT1239</t>
   </si>
   <si>
-    <t>DXLY4265</t>
-  </si>
-  <si>
     <t>MP04CT1240</t>
   </si>
   <si>
-    <t>DXLY4266</t>
-  </si>
-  <si>
-    <t>name</t>
+    <t>TATA</t>
+  </si>
+  <si>
+    <t>Mahindra</t>
+  </si>
+  <si>
+    <t>Harrier</t>
+  </si>
+  <si>
+    <t>Nexon</t>
+  </si>
+  <si>
+    <t>Bolero</t>
+  </si>
+  <si>
+    <t>XUV 700</t>
+  </si>
+  <si>
+    <t>Range Rover</t>
+  </si>
+  <si>
+    <t>ASK-01</t>
+  </si>
+  <si>
+    <t>ASK-02</t>
+  </si>
+  <si>
+    <t>ASK-12</t>
+  </si>
+  <si>
+    <t>BSK-01</t>
+  </si>
+  <si>
+    <t>ASK-04</t>
+  </si>
+  <si>
+    <t>BSK-02</t>
+  </si>
+  <si>
+    <t>gmail</t>
+  </si>
+  <si>
+    <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>test3@gmail.com</t>
+  </si>
+  <si>
+    <t>Vehicle Registration Number</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>isAc</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +152,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,13 +182,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,11 +499,12 @@
     <col min="6" max="6" width="17.26953125" customWidth="1"/>
     <col min="7" max="7" width="16.54296875" customWidth="1"/>
     <col min="8" max="8" width="19.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -464,36 +513,48 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <v>32000</v>
@@ -504,22 +565,34 @@
       <c r="H2">
         <v>6</v>
       </c>
+      <c r="I2">
+        <v>2020</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>300</v>
+      </c>
+      <c r="L2" s="2">
+        <v>45370</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F3">
         <v>32001</v>
@@ -530,22 +603,34 @@
       <c r="H3">
         <v>7</v>
       </c>
+      <c r="I3">
+        <v>2021</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>3000</v>
+      </c>
+      <c r="L3" s="2">
+        <v>45370</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F4">
         <v>32002</v>
@@ -556,22 +641,34 @@
       <c r="H4">
         <v>8</v>
       </c>
+      <c r="I4">
+        <v>2022</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>4500</v>
+      </c>
+      <c r="L4" s="2">
+        <v>45370</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>32003</v>
@@ -582,22 +679,34 @@
       <c r="H5">
         <v>9</v>
       </c>
+      <c r="I5">
+        <v>2021</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>2300</v>
+      </c>
+      <c r="L5" s="2">
+        <v>45370</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <v>32004</v>
@@ -608,22 +717,34 @@
       <c r="H6">
         <v>10</v>
       </c>
+      <c r="I6">
+        <v>2020</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>6755</v>
+      </c>
+      <c r="L6" s="2">
+        <v>45370</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F7">
         <v>32005</v>
@@ -634,22 +755,34 @@
       <c r="H7">
         <v>11</v>
       </c>
+      <c r="I7">
+        <v>2019</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>4356</v>
+      </c>
+      <c r="L7" s="2">
+        <v>45370</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F8">
         <v>32006</v>
@@ -659,10 +792,31 @@
       </c>
       <c r="H8">
         <v>12</v>
+      </c>
+      <c r="I8">
+        <v>2023</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>24674</v>
+      </c>
+      <c r="L8" s="2">
+        <v>45370</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4686FBCF-1CFC-44CB-B4E2-A0554B35C88B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{07DF3807-7E13-4D5B-B42A-596C4C936F9D}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{362D8BD3-E801-4F95-A31F-6962E2B81751}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{0D1E4963-84E1-458B-B97F-5056DDB2D064}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{B90B04D1-9F46-4C94-BA89-6D5B5C53ACE0}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{177446FB-FAB6-43EE-B700-2A98CD33FF70}"/>
+    <hyperlink ref="A7" r:id="rId7" xr:uid="{9A566EE7-67EB-4CE6-BE3B-B25A668887FD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed frv code in addNewOwner page
</commit_message>
<xml_diff>
--- a/resources/cars.xlsx
+++ b/resources/cars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Techidol solutions\CRM\crm_dashboard\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35E0617-3B1C-4187-9B85-7A6A02A7C82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FECDEB-E86A-4ED6-A472-3FD071A8E052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Brand</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>FRV code</t>
-  </si>
-  <si>
     <t>Rent</t>
   </si>
   <si>
@@ -93,24 +90,6 @@
     <t>Range Rover</t>
   </si>
   <si>
-    <t>ASK-01</t>
-  </si>
-  <si>
-    <t>ASK-02</t>
-  </si>
-  <si>
-    <t>ASK-12</t>
-  </si>
-  <si>
-    <t>BSK-01</t>
-  </si>
-  <si>
-    <t>ASK-04</t>
-  </si>
-  <si>
-    <t>BSK-02</t>
-  </si>
-  <si>
     <t>gmail</t>
   </si>
   <si>
@@ -136,6 +115,30 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>MP04CT1241</t>
+  </si>
+  <si>
+    <t>MP04CT1242</t>
+  </si>
+  <si>
+    <t>MP04CT1243</t>
+  </si>
+  <si>
+    <t>MP04CT1244</t>
+  </si>
+  <si>
+    <t>MP04CT1245</t>
+  </si>
+  <si>
+    <t>MP04CT1246</t>
+  </si>
+  <si>
+    <t>MP04CT1247</t>
+  </si>
+  <si>
+    <t>MP04CT1248</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,16 +498,15 @@
     <col min="2" max="2" width="14.08984375" customWidth="1"/>
     <col min="3" max="3" width="15.36328125" customWidth="1"/>
     <col min="4" max="4" width="26.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="19.26953125" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="19.26953125" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -513,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -525,284 +527,540 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>32000</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>2020</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>300</v>
+      </c>
+      <c r="K2" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>32001</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>2021</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>3000</v>
+      </c>
+      <c r="K3" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>32002</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>2022</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>4500</v>
+      </c>
+      <c r="K4" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>32003</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>2021</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2300</v>
+      </c>
+      <c r="K5" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>32004</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>2020</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>6755</v>
+      </c>
+      <c r="K6" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>32005</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>2019</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>4356</v>
+      </c>
+      <c r="K7" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>32006</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>2023</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>24674</v>
+      </c>
+      <c r="K8" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>32007</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>2023.6666666666699</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>29847.333333333299</v>
+      </c>
+      <c r="K9" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>32008</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>2025.1666666666699</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>38806.833333333299</v>
+      </c>
+      <c r="K10" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>32009</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>2026.6666666666699</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>47766.333333333299</v>
+      </c>
+      <c r="K11" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="J1" t="s">
+      <c r="E12">
+        <v>32010</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>2028.1666666666699</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>56725.833333333299</v>
+      </c>
+      <c r="K12" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="E13">
+        <v>32011</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <v>2029.6666666666699</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>65685.333333333299</v>
+      </c>
+      <c r="K13" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
         <v>35</v>
       </c>
-      <c r="L1" t="s">
+      <c r="E14">
+        <v>32012</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>18</v>
+      </c>
+      <c r="H14">
+        <v>2031.1666666666699</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>74644.833333333299</v>
+      </c>
+      <c r="K14" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E15">
+        <v>32013</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>19</v>
+      </c>
+      <c r="H15">
+        <v>2032.6666666666699</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>83604.333333333299</v>
+      </c>
+      <c r="K15" s="2">
+        <v>45370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2">
-        <v>32000</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>2020</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>300</v>
-      </c>
-      <c r="L2" s="2">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3">
-        <v>32001</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>7</v>
-      </c>
-      <c r="I3">
-        <v>2021</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>3000</v>
-      </c>
-      <c r="L3" s="2">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>32014</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4">
-        <v>32002</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>8</v>
-      </c>
-      <c r="I4">
-        <v>2022</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>4500</v>
-      </c>
-      <c r="L4" s="2">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5">
-        <v>32003</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>9</v>
-      </c>
-      <c r="I5">
-        <v>2021</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>2300</v>
-      </c>
-      <c r="L5" s="2">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6">
-        <v>32004</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="I6">
-        <v>2020</v>
-      </c>
-      <c r="J6" t="b">
+      <c r="H16">
+        <v>2034.1666666666699</v>
+      </c>
+      <c r="I16" t="b">
         <v>0</v>
       </c>
-      <c r="K6">
-        <v>6755</v>
-      </c>
-      <c r="L6" s="2">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7">
-        <v>32005</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>11</v>
-      </c>
-      <c r="I7">
-        <v>2019</v>
-      </c>
-      <c r="J7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>4356</v>
-      </c>
-      <c r="L7" s="2">
-        <v>45370</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8">
-        <v>32006</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>12</v>
-      </c>
-      <c r="I8">
-        <v>2023</v>
-      </c>
-      <c r="J8" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>24674</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="J16">
+        <v>92563.833333333299</v>
+      </c>
+      <c r="K16" s="2">
         <v>45370</v>
       </c>
     </row>
@@ -816,6 +1074,14 @@
     <hyperlink ref="A6" r:id="rId5" xr:uid="{B90B04D1-9F46-4C94-BA89-6D5B5C53ACE0}"/>
     <hyperlink ref="A8" r:id="rId6" xr:uid="{177446FB-FAB6-43EE-B700-2A98CD33FF70}"/>
     <hyperlink ref="A7" r:id="rId7" xr:uid="{9A566EE7-67EB-4CE6-BE3B-B25A668887FD}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{298DE624-3E26-4E61-ACA4-03B057F5485D}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{621694F6-646E-4966-BFC4-C3F10F0D0AE0}"/>
+    <hyperlink ref="A15" r:id="rId10" display="test3@gmail.com" xr:uid="{27ED2EC7-A684-4078-B470-AD05E0232E22}"/>
+    <hyperlink ref="A11" r:id="rId11" xr:uid="{2DAC6BFB-8F82-409B-A950-E6312E1EC995}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{9BEBE5D4-011E-4916-807F-6B10874F58A0}"/>
+    <hyperlink ref="A10" r:id="rId13" xr:uid="{1D0DAE7D-A752-43F4-8FBD-4AE429C7B1C0}"/>
+    <hyperlink ref="A13" r:id="rId14" xr:uid="{09219576-2CA4-4877-B8DE-C646E14BA6D4}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{8930E7E1-F84C-49FC-9842-4C1FF825DF77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cars excel file changed
</commit_message>
<xml_diff>
--- a/resources/cars.xlsx
+++ b/resources/cars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Techidol solutions\CRM\crm_dashboard\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998B23C4-F59A-4735-A5F0-64762199F9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F8B61F-B9B4-43B6-A8D9-C4EF3F18BCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>Range Rover</t>
   </si>
   <si>
-    <t>gmail</t>
-  </si>
-  <si>
     <t>test1@gmail.com</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>Rent Charges</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -473,9 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -489,7 +487,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -498,21 +496,21 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -535,7 +533,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -558,7 +556,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -581,7 +579,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -604,7 +602,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -627,7 +625,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -650,7 +648,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -673,7 +671,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -682,7 +680,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -696,7 +694,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -705,7 +703,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -719,7 +717,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -728,7 +726,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -742,7 +740,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -751,7 +749,7 @@
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -765,7 +763,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -774,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -788,7 +786,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -797,7 +795,7 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -811,7 +809,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -820,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -834,7 +832,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -843,7 +841,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16">
         <v>0</v>

</xml_diff>